<commit_message>
added better reporting using HTMl and included Dataprovider and screenshot
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/simple.xlsx
+++ b/src/test/resources/testdata/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="tc_01" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,13 @@
     <sheet name="tc_05" sheetId="6" r:id="rId5"/>
     <sheet name="tc_06" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:P24"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:R17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Abhigya</t>
-  </si>
-  <si>
     <t>Rahul</t>
   </si>
   <si>
@@ -45,12 +42,24 @@
   <si>
     <t>Suresh</t>
   </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>q34234</t>
+  </si>
+  <si>
+    <t>dfsdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,10 +182,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,7 +216,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -384,16 +391,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A4" sqref="A4:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,12 +411,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>8744954505</v>
       </c>
       <c r="B2">
         <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -415,16 +433,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -445,17 +494,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -476,17 +525,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -507,48 +556,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,9 +574,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>12345</v>

</xml_diff>

<commit_message>
Started Testing on ZOHO.com
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/simple.xlsx
+++ b/src/test/resources/testdata/simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="5610"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="tc_01" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="tc_04" sheetId="5" r:id="rId4"/>
     <sheet name="tc_05" sheetId="6" r:id="rId5"/>
     <sheet name="tc_06" sheetId="7" r:id="rId6"/>
+    <sheet name="testData" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
   <oleSize ref="A1:R17"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -49,10 +50,37 @@
     <t>password</t>
   </si>
   <si>
-    <t>q34234</t>
-  </si>
-  <si>
-    <t>dfsdf</t>
+    <t>tc_02</t>
+  </si>
+  <si>
+    <t>tc_01</t>
+  </si>
+  <si>
+    <t>esdf</t>
+  </si>
+  <si>
+    <t>sdwerwe</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>qwewer</t>
+  </si>
+  <si>
+    <t>fsfsd</t>
+  </si>
+  <si>
+    <t>dsdfsdf</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastaname</t>
   </si>
 </sst>
 </file>
@@ -392,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,14 +445,6 @@
       </c>
       <c r="B2">
         <v>12345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -585,4 +605,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>8744954505</v>
+      </c>
+      <c r="B3">
+        <v>12123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed xpath used to find CRM link in homepage
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/simple.xlsx
+++ b/src/test/resources/testdata/simple.xlsx
@@ -16,12 +16,11 @@
     <sheet name="testData" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:R17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -81,19 +80,35 @@
   </si>
   <si>
     <t>lastaname</t>
+  </si>
+  <si>
+    <t>verifyLoginWithValidCred</t>
+  </si>
+  <si>
+    <t>w2ajava@way2automation.com</t>
+  </si>
+  <si>
+    <t>Tcs@12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,13 +128,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,10 +630,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,7 +708,31 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>